<commit_message>
Add json files for raw data
</commit_message>
<xml_diff>
--- a/src/assets/Reference.xlsx
+++ b/src/assets/Reference.xlsx
@@ -5,17 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AngularApps\E-Commerce Wesite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AngularApps\E-Commerce Wesite\E-Commerce\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640DB33A-5916-41FB-9AFA-0E0EF2F684CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8C6CAD-5BDC-4267-A5A3-41E63CB437D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Drinks" sheetId="3" r:id="rId2"/>
+    <sheet name="Games" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>CLOTHS</t>
   </si>
@@ -157,6 +159,15 @@
   </si>
   <si>
     <t>RAM:8GB DDR4 PROCESSOR:INTEL-10i 9TH GENERATION HDD:1TB HDD 256GB SSD OS:WINDOWS 10 PRICE: 60,199</t>
+  </si>
+  <si>
+    <t>Followers</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Available Quantity</t>
   </si>
 </sst>
 </file>
@@ -221,10 +232,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,4 +750,396 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59F07BF-B1FE-4E99-8AC3-67146195986F}">
+  <dimension ref="C3:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>250</v>
+      </c>
+      <c r="F4" s="5">
+        <v>24456</v>
+      </c>
+      <c r="I4" t="str">
+        <f>" { 'id' : "&amp;C4&amp;", 'Drink' : '"&amp;D4&amp;"', 'Availability' : "&amp;F4&amp;", 'Price' : "&amp;E4&amp;" },"</f>
+        <v xml:space="preserve"> { 'id' : 1, 'Drink' : 'Wine', 'Availability' : 24456, 'Price' : 250 },</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5" s="5">
+        <v>3456</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" ref="I5:I13" si="0">" { 'id' : "&amp;C5&amp;", 'Drink' : '"&amp;D5&amp;"', 'Availability' : "&amp;F5&amp;", 'Price' : "&amp;E5&amp;" },"</f>
+        <v xml:space="preserve"> { 'id' : 2, 'Drink' : 'Coffee', 'Availability' : 3456, 'Price' : 50 },</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="F6" s="5">
+        <v>2456</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> { 'id' : 3, 'Drink' : 'Lemonade', 'Availability' : 2456, 'Price' : 30 },</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7">
+        <v>40</v>
+      </c>
+      <c r="F7" s="5">
+        <v>8743</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> { 'id' : 4, 'Drink' : 'Iced Tea', 'Availability' : 8743, 'Price' : 40 },</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>60</v>
+      </c>
+      <c r="F8" s="5">
+        <v>7963</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> { 'id' : 5, 'Drink' : 'Hot Chocolate', 'Availability' : 7963, 'Price' : 60 },</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
+      </c>
+      <c r="F9" s="5">
+        <v>6437</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> { 'id' : 6, 'Drink' : 'Juice', 'Availability' : 6437, 'Price' : 30 },</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>40</v>
+      </c>
+      <c r="F10" s="5">
+        <v>8453</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> { 'id' : 7, 'Drink' : 'Milkshake', 'Availability' : 8453, 'Price' : 40 },</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11" s="5">
+        <v>7357</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> { 'id' : 8, 'Drink' : 'Water', 'Availability' : 7357, 'Price' : 20 },</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12" s="5">
+        <v>8442</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> { 'id' : 9, 'Drink' : 'Tea', 'Availability' : 8442, 'Price' : 10 },</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13">
+        <v>140</v>
+      </c>
+      <c r="F13" s="5">
+        <v>7457</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> { 'id' : 10, 'Drink' : 'Beer', 'Availability' : 7457, 'Price' : 140 },</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0F7EE7-84A9-4D72-A8D5-4B40F7FE4C64}">
+  <dimension ref="C2:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5">
+        <v>70577</v>
+      </c>
+      <c r="F3" t="str">
+        <f>"{ 'id' = "&amp;C3&amp;", 'Game' : "&amp;D3&amp;", 'Followers' : "&amp;E3&amp;"},"</f>
+        <v>{ 'id' = 1, 'Game' : Soccer, 'Followers' : 70577},</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5">
+        <v>20744</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F13" si="0">"{ 'id' = "&amp;C4&amp;", 'Game' : "&amp;D4&amp;", 'Followers' : "&amp;E4&amp;"},"</f>
+        <v>{ 'id' = 2, 'Game' : Basketball, 'Followers' : 20744},</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="5">
+        <v>10003</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'id' = 3, 'Game' : Tennis, 'Followers' : 10003},</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="3">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5">
+        <v>23992</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'id' = 4, 'Game' : Baseball, 'Followers' : 23992},</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="5">
+        <v>3456</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'id' = 5, 'Game' : Golf, 'Followers' : 3456},</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="3">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1205478</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'id' = 6, 'Game' : Running, 'Followers' : 1205478},</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="3">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="5">
+        <v>50944</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'id' = 7, 'Game' : Volleyball, 'Followers' : 50944},</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="3">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="5">
+        <v>126087</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'id' = 8, 'Game' : Badminton, 'Followers' : 126087},</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="3">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="5">
+        <v>256843</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'id' = 9, 'Game' : Swimming, 'Followers' : 256843},</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="3">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="5">
+        <v>177435</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'id' = 10, 'Game' : Boxing, 'Followers' : 177435},</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="3">
+        <v>11</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="5">
+        <v>198436</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'id' = 11, 'Game' : Table Tennis, 'Followers' : 198436},</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>